<commit_message>
Adapted for practice 190224SS
- Add some missing values
</commit_message>
<xml_diff>
--- a/psu_intuss.xlsx
+++ b/psu_intuss.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/surasaksangkhathat/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F02CD48-DE2E-914B-84C9-91CFFA05788C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1516F9E-CE35-3143-AFBD-A9E93E8FF184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="H136" sqref="H136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14412,9 +14412,6 @@
       <c r="G136">
         <v>12.5</v>
       </c>
-      <c r="H136">
-        <v>57</v>
-      </c>
       <c r="I136">
         <v>0</v>
       </c>
@@ -14724,9 +14721,6 @@
       <c r="G139">
         <v>8</v>
       </c>
-      <c r="H139">
-        <v>16</v>
-      </c>
       <c r="I139">
         <v>0</v>
       </c>
@@ -15157,9 +15151,6 @@
       <c r="G144">
         <v>14</v>
       </c>
-      <c r="H144">
-        <v>40</v>
-      </c>
       <c r="I144">
         <v>0</v>
       </c>
@@ -15486,9 +15477,6 @@
       </c>
       <c r="G147">
         <v>8.6</v>
-      </c>
-      <c r="H147">
-        <v>12</v>
       </c>
       <c r="I147">
         <v>0</v>

</xml_diff>